<commit_message>
Deleted fill base data sql script and updated Workbook and .gitignore
</commit_message>
<xml_diff>
--- a/project_docs/Workbook.xlsx
+++ b/project_docs/Workbook.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saharmohamedali/groupproject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saharmohamedali/groupproject/Ragnar/project_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prioriy List" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>As a Network Management Engineer I want to have a range of  "drill down" capabilities on my Graphical Representations (e.g. Click on a Cell ID, see the associated failures, click on a failure, see the details etc.) OR (click on a Cause Class, drill down to the Cells affected, show the total duration of failures etc. etc.)</t>
   </si>
@@ -263,6 +263,15 @@
   </si>
   <si>
     <t>Input</t>
+  </si>
+  <si>
+    <t>Researching</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Dimitar &amp; Ciaran</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -427,6 +436,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +726,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -747,8 +765,12 @@
       <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
@@ -760,8 +782,12 @@
       <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
@@ -773,8 +799,12 @@
       <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
@@ -786,10 +816,14 @@
       <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1102,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data upload and import fully working
</commit_message>
<xml_diff>
--- a/project_docs/Workbook.xlsx
+++ b/project_docs/Workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="prioriy List" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'prioriy List'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'prioriy List'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'prioriy List'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="214">
   <si>
     <t>Priority</t>
   </si>
@@ -50,18 +51,21 @@
     <t>Carl</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>As the System Administrator I want to have incoming records checked for consistency (i.e. valid date / time values, valid MNC / MCC combinations, valid Event IDs, Cause Codes etc.) and have erroneous records highlighted and excluded</t>
+  </si>
+  <si>
+    <t>As the System Administrator I want to be able to assign an Id and password to each User type (i.e. Customer Service Rep., Support Engineer, Network Management Engineer)</t>
+  </si>
+  <si>
+    <t>Dimitar &amp; Ciaran</t>
+  </si>
+  <si>
     <t>Researching</t>
   </si>
   <si>
-    <t>As the System Administrator I want to have incoming records checked for consistency (i.e. valid date / time values, valid MNC / MCC combinations, valid Event IDs, Cause Codes etc.) and have erroneous records highlighted and excluded</t>
-  </si>
-  <si>
-    <t>As the System Administrator I want to be able to assign an Id and password to each User type (i.e. Customer Service Rep., Support Engineer, Network Management Engineer)</t>
-  </si>
-  <si>
-    <t>Dimitar &amp; Ciaran</t>
-  </si>
-  <si>
     <t>As Customer Service Rep. I want to display, for a given affected IMSI, the Event ID and Cause Code for any / all failures affecting that IMSI</t>
   </si>
   <si>
@@ -126,9 +130,6 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>Review the initial Query List</t>
@@ -678,7 +679,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -730,12 +731,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -838,6 +833,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -851,19 +850,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="10" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -886,10 +881,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -898,16 +889,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -922,7 +917,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -998,324 +993,329 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6760563380282"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5962441314554"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="104.183098591549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.830985915493"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="12.0234741784038"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7089201877934"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8544600938967"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="114.014084507042"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="29.6384976525822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.962441314554"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="13.075117370892"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" customFormat="false" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" customFormat="false" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B14" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B15" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B16" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="n">
+      <c r="B17" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B20" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>
@@ -1337,19 +1337,19 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="78.0328638497653"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.8262910798122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.3521126760563"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.868544600939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>3</v>
@@ -1360,13 +1360,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,10 +1374,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1385,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0"/>
     </row>
@@ -1394,10 +1394,10 @@
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,18 +1428,18 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.2910798122066"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="73.112676056338"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.3521126760563"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="54.3896713615023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.131455399061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.8262910798122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.0046948356808"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="80.018779342723"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.4272300469484"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="59.5258215962441"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.0140845070423"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="12.868544600939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,15 +1676,14 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="C20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1724,17 +1723,17 @@
   </sheetPr>
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I156" activeCellId="0" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6431924882629"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.037558685446"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.6009389671362"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.50704225352113"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6009389671362"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2910798122066"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8450704225352"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.5117370892019"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.96244131455399"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5117370892019"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,25 +1751,25 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1783,7 +1782,7 @@
         <v>87</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>8</v>
@@ -1793,7 +1792,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1829,7 +1828,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>8</v>
@@ -1844,7 +1843,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1905,7 +1904,7 @@
         <v>109</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>1</v>
@@ -1922,7 +1921,7 @@
         <v>109</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>8</v>
@@ -1939,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1</v>
@@ -1956,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>8</v>
@@ -1973,7 +1972,7 @@
         <v>109</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>1</v>
@@ -1990,7 +1989,7 @@
         <v>109</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>8</v>
@@ -2007,7 +2006,7 @@
         <v>116</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
@@ -2024,7 +2023,7 @@
         <v>116</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>8</v>
@@ -2038,10 +2037,10 @@
         <v>118</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>1</v>
@@ -2055,10 +2054,10 @@
         <v>119</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>8</v>
@@ -2075,7 +2074,7 @@
         <v>87</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>1</v>
@@ -2092,7 +2091,7 @@
         <v>87</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>8</v>
@@ -2112,7 +2111,7 @@
         <v>6</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>1</v>
@@ -2122,14 +2121,14 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>124</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>125</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>1</v>
@@ -2146,7 +2145,7 @@
         <v>6</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>1</v>
@@ -2156,7 +2155,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="19" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2169,12 +2168,12 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2199,7 +2198,7 @@
         <v>109</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>4</v>
@@ -2216,7 +2215,7 @@
         <v>6</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>8</v>
@@ -2233,7 +2232,7 @@
         <v>109</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>4</v>
@@ -2250,7 +2249,7 @@
         <v>116</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>6</v>
@@ -2264,10 +2263,10 @@
         <v>139</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>4</v>
@@ -2284,7 +2283,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>2</v>
@@ -2304,7 +2303,7 @@
         <v>6</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>1</v>
@@ -2321,7 +2320,7 @@
         <v>116</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>1</v>
@@ -2387,7 +2386,7 @@
         <v>109</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H72" s="0" t="n">
         <v>1</v>
@@ -2404,7 +2403,7 @@
         <v>109</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H73" s="0" t="n">
         <v>1</v>
@@ -2421,7 +2420,7 @@
         <v>6</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H74" s="0" t="n">
         <v>1</v>
@@ -2438,7 +2437,7 @@
         <v>6</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H75" s="0" t="n">
         <v>1</v>
@@ -2455,7 +2454,7 @@
         <v>109</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H76" s="0" t="n">
         <v>1</v>
@@ -2472,7 +2471,7 @@
         <v>109</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H77" s="0" t="n">
         <v>1</v>
@@ -2489,7 +2488,7 @@
         <v>116</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H78" s="0" t="n">
         <v>1</v>
@@ -2506,7 +2505,7 @@
         <v>116</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H79" s="0" t="n">
         <v>1</v>
@@ -2520,10 +2519,10 @@
         <v>156</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H80" s="0" t="n">
         <v>1</v>
@@ -2537,10 +2536,10 @@
         <v>157</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H81" s="0" t="n">
         <v>1</v>
@@ -2557,7 +2556,7 @@
         <v>87</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H82" s="0" t="n">
         <v>1</v>
@@ -2574,7 +2573,7 @@
         <v>87</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H83" s="0" t="n">
         <v>1</v>
@@ -2584,8 +2583,8 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18" t="s">
+      <c r="A85" s="19"/>
+      <c r="B85" s="19" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2640,7 +2639,7 @@
         <v>109</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H96" s="0" t="n">
         <v>4</v>
@@ -2657,7 +2656,7 @@
         <v>6</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H97" s="0" t="n">
         <v>4</v>
@@ -2674,7 +2673,7 @@
         <v>109</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H98" s="0" t="n">
         <v>4</v>
@@ -2691,7 +2690,7 @@
         <v>116</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H99" s="0" t="n">
         <v>4</v>
@@ -2708,7 +2707,7 @@
         <v>6</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H100" s="0" t="n">
         <v>4</v>
@@ -2722,10 +2721,10 @@
         <v>174</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H101" s="0" t="n">
         <v>4</v>
@@ -2798,7 +2797,7 @@
         <v>6</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H109" s="0" t="n">
         <v>2</v>
@@ -2842,10 +2841,10 @@
         <v>189</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H117" s="0" t="n">
         <v>3</v>
@@ -2865,7 +2864,7 @@
         <v>109</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H126" s="0" t="n">
         <v>1</v>
@@ -2885,7 +2884,7 @@
         <v>87</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H127" s="0" t="n">
         <v>1</v>
@@ -2938,7 +2937,7 @@
         <v>109</v>
       </c>
       <c r="G136" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H136" s="0" t="n">
         <v>3</v>
@@ -2955,7 +2954,7 @@
         <v>6</v>
       </c>
       <c r="G137" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H137" s="0" t="n">
         <v>6</v>
@@ -2972,7 +2971,7 @@
         <v>109</v>
       </c>
       <c r="G138" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H138" s="0" t="n">
         <v>3</v>
@@ -2989,7 +2988,7 @@
         <v>6</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H139" s="0" t="n">
         <v>8</v>
@@ -3006,7 +3005,7 @@
         <v>116</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H141" s="0" t="n">
         <v>4</v>
@@ -3020,10 +3019,10 @@
         <v>205</v>
       </c>
       <c r="F142" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H142" s="0" t="n">
         <v>4</v>
@@ -3060,7 +3059,7 @@
         <v>87</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H145" s="0" t="n">
         <v>1</v>
@@ -3085,7 +3084,7 @@
         <v>109</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H148" s="0" t="n">
         <v>4</v>
@@ -3100,8 +3099,8 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="18"/>
-      <c r="B152" s="18"/>
+      <c r="A152" s="19"/>
+      <c r="B152" s="19"/>
       <c r="H152" s="0" t="n">
         <f aca="false">SUM(H148,H148,H145,H143,H142,H141,H139,H138,H137,H136,H126,H127,H117,H109,H108,H104,H102,H101,H100,H99,H98,H97,H96,H72,H73,H74,H75,H76,H77,H78,H79,H80,H81,H82,H83,H59,H58,H56,H55,H54,H53,H52,H51,H41,H40,H39,H37,H36,H35,H34,H33,H32,H31,H30,H29,H28,H27,H26,H11,H5)</f>
         <v>205</v>

</xml_diff>